<commit_message>
Version 2.1.1 minor fix bug
</commit_message>
<xml_diff>
--- a/DB/Термометры медицинские.xlsx
+++ b/DB/Термометры медицинские.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\V2_test\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\printing\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99515D06-2E5D-49AD-89F7-8E3380966CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267701E8-C534-4001-A975-982B32F239DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="540" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>№ ГРСИ</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Величина погрешности 3</t>
+  </si>
+  <si>
+    <t>23811-13</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,42 +643,57 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10">
-        <v>32</v>
-      </c>
-      <c r="C4" s="6">
-        <v>43</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.1</v>
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>43.9</v>
+      </c>
+      <c r="E4">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>43.9</v>
+      </c>
+      <c r="J4">
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="10">
         <v>32</v>
       </c>
       <c r="C5" s="6">
-        <v>43.9</v>
-      </c>
-      <c r="D5" s="6">
+        <v>43</v>
+      </c>
+      <c r="D5" s="7">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="10">
         <v>32</v>
       </c>
       <c r="C6" s="6">
-        <v>42.9</v>
+        <v>43.9</v>
       </c>
       <c r="D6" s="6">
         <v>0.1</v>
@@ -683,13 +701,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="10">
         <v>32</v>
       </c>
       <c r="C7" s="6">
-        <v>42</v>
+        <v>42.9</v>
       </c>
       <c r="D7" s="6">
         <v>0.1</v>
@@ -697,7 +715,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="10">
         <v>32</v>
@@ -709,9 +727,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>8</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="10">
         <v>32</v>
@@ -720,6 +738,20 @@
         <v>42</v>
       </c>
       <c r="D9" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>